<commit_message>
fixed indexed issues, made work for non clustered joints
</commit_message>
<xml_diff>
--- a/MilestoneThreeRubric.xlsx
+++ b/MilestoneThreeRubric.xlsx
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="9">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -568,23 +568,23 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B11" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B13" s="3">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First thoughts on lerping
</commit_message>
<xml_diff>
--- a/MilestoneThreeRubric.xlsx
+++ b/MilestoneThreeRubric.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Peter Farber</t>
   </si>
@@ -56,13 +56,19 @@
     <t>add interpolation between keyframes for smooth transition</t>
   </si>
   <si>
-    <t>add in normal mapping</t>
-  </si>
-  <si>
     <t>add indexed joint indicies back in</t>
   </si>
   <si>
     <t>will not be dependant on only having 4 joints</t>
+  </si>
+  <si>
+    <t>interpolate between 2 animations</t>
+  </si>
+  <si>
+    <t>add in normal mapping with specular map</t>
+  </si>
+  <si>
+    <t>be able to roate model</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,13 +538,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="7">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -546,7 +552,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -555,36 +561,55 @@
         <v>10</v>
       </c>
       <c r="B9" s="9">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" s="9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B15" s="3">
+        <f>SUM(B7:B13)</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>